<commit_message>
avancé phase 1 termiée
</commit_message>
<xml_diff>
--- a/Business/2-etude marché/tarifs_lignes.xlsx
+++ b/Business/2-etude marché/tarifs_lignes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\izyGO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\izyGO\Business\2-etude marché\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C8950D-0430-4F95-9B7E-1426480DBFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3EA78B-15E3-47A6-88C8-FEA52FB4C16B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarifs_lignes" sheetId="1" r:id="rId1"/>
     <sheet name="Villes" sheetId="2" r:id="rId2"/>
+    <sheet name="calcul" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t xml:space="preserve">AT TRANSPORT </t>
   </si>
@@ -154,6 +155,39 @@
   </si>
   <si>
     <t>Bangolo</t>
+  </si>
+  <si>
+    <t>Montant ticket</t>
+  </si>
+  <si>
+    <t>Total tickets vendu</t>
+  </si>
+  <si>
+    <t>Comission Total</t>
+  </si>
+  <si>
+    <t>Commission Payement</t>
+  </si>
+  <si>
+    <t>Comission Demarcheur</t>
+  </si>
+  <si>
+    <t>Vendu Site</t>
+  </si>
+  <si>
+    <t>Benefice Demarcheur</t>
+  </si>
+  <si>
+    <t>Benefice Payement</t>
+  </si>
+  <si>
+    <t>Benefice Total</t>
+  </si>
+  <si>
+    <t>Vendu Demarcheur</t>
+  </si>
+  <si>
+    <t>Gagné/jour</t>
   </si>
 </sst>
 </file>
@@ -187,7 +221,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +264,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -243,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -272,15 +330,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +684,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +719,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -672,7 +734,7 @@
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -685,7 +747,7 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
@@ -697,7 +759,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
@@ -709,7 +771,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -720,7 +782,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
@@ -729,7 +791,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -741,7 +803,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
@@ -753,7 +815,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
@@ -765,7 +827,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
@@ -777,7 +839,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
@@ -789,7 +851,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
@@ -800,8 +862,8 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -813,7 +875,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -861,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E016C6C-7C50-45D1-B8D9-42134E92566A}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,4 +1227,786 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B265A3FA-6A83-4FD6-8640-BE8DAE70E0F1}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1500</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2,C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0.15</v>
+      </c>
+      <c r="F2">
+        <v>0.03</v>
+      </c>
+      <c r="G2">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <f>PRODUCT(A2,E2,D2)</f>
+        <v>225</v>
+      </c>
+      <c r="I2">
+        <f>PRODUCT(A2,G2,C2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>PRODUCT(D2,F2,A2)</f>
+        <v>45</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IMSUB(IMSUB(H2,I2),J2)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">SUM(B3,C3)</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0.03</v>
+      </c>
+      <c r="G3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H5" si="1">PRODUCT(A3,E3,D3)</f>
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="2">PRODUCT(A3,G3,C3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J19" si="3">PRODUCT(D3,F3,A3)</f>
+        <v>60</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K5" si="4">IMSUB(IMSUB(H3,I3),J3)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2500</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.03</v>
+      </c>
+      <c r="G4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5">
+        <v>0.03</v>
+      </c>
+      <c r="G5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3500</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6" si="5">SUM(B6,C6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+      <c r="F6">
+        <v>0.03</v>
+      </c>
+      <c r="G6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6" si="6">PRODUCT(A6,E6,D6)</f>
+        <v>350</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6" si="7">PRODUCT(A6,G6,C6)</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6" si="8">IMSUB(IMSUB(H6,I6),J6)</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4000</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>SUM(B7,C7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.03</v>
+      </c>
+      <c r="G7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H7">
+        <f>PRODUCT(A7,E7,D7)</f>
+        <v>400</v>
+      </c>
+      <c r="I7">
+        <f>PRODUCT(A7,G7,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IMSUB(IMSUB(H7,I7),J7)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4500</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>SUM(B8,C8)</f>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0.03</v>
+      </c>
+      <c r="G8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H8">
+        <f>PRODUCT(A8,E8,D8)</f>
+        <v>450</v>
+      </c>
+      <c r="I8">
+        <f>PRODUCT(A8,G8,C8)</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="K8" t="str">
+        <f>IMSUB(IMSUB(H8,I8),J8)</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5000</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>SUM(B9,C9)</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>0.03</v>
+      </c>
+      <c r="G9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H9">
+        <f>PRODUCT(A9,E9,D9)</f>
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <f>PRODUCT(A9,G9,C9)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IMSUB(IMSUB(H9,I9),J9)</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5500</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>SUM(B10,C10)</f>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0.03</v>
+      </c>
+      <c r="G10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H10">
+        <f>PRODUCT(A10,E10,D10)</f>
+        <v>550</v>
+      </c>
+      <c r="I10">
+        <f>PRODUCT(A10,G10,C10)</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>165</v>
+      </c>
+      <c r="K10" t="str">
+        <f>IMSUB(IMSUB(H10,I10),J10)</f>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6000</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D12" si="9">SUM(B11,C11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11">
+        <v>0.03</v>
+      </c>
+      <c r="G11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H12" si="10">PRODUCT(A11,E11,D11)</f>
+        <v>600</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I12" si="11">PRODUCT(A11,G11,C11)</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" ref="K11:K12" si="12">IMSUB(IMSUB(H11,I11),J11)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6500</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.03</v>
+      </c>
+      <c r="G12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="10"/>
+        <v>650</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="12"/>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7000</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D14" si="13">SUM(B13,C13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <v>0.03</v>
+      </c>
+      <c r="G13">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H14" si="14">PRODUCT(A13,E13,D13)</f>
+        <v>700</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I14" si="15">PRODUCT(A13,G13,C13)</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" ref="K13:K14" si="16">IMSUB(IMSUB(H13,I13),J13)</f>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7500</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <v>0.03</v>
+      </c>
+      <c r="G14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="14"/>
+        <v>750</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="16"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8000</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D19" si="17">SUM(B15,C15)</f>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>0.03</v>
+      </c>
+      <c r="G15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H19" si="18">PRODUCT(A15,E15,D15)</f>
+        <v>800</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I19" si="19">PRODUCT(A15,G15,C15)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" ref="K15:K19" si="20">IMSUB(IMSUB(H15,I15),J15)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8500</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+      <c r="F16">
+        <v>0.03</v>
+      </c>
+      <c r="G16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="18"/>
+        <v>850</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="20"/>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9000</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0.1</v>
+      </c>
+      <c r="F17">
+        <v>0.03</v>
+      </c>
+      <c r="G17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="18"/>
+        <v>900</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="20"/>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>9500</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+      <c r="F18">
+        <v>0.03</v>
+      </c>
+      <c r="G18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="18"/>
+        <v>950</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>285</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="20"/>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.1</v>
+      </c>
+      <c r="F19">
+        <v>0.03</v>
+      </c>
+      <c r="G19">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="18"/>
+        <v>1000</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="20"/>
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>